<commit_message>
Updating decimal issues for SO5
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDriver/TestRevenue/Test.xlsx
+++ b/src/test/resources/TestDriver/TestRevenue/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arahmed\OneDrive - SS&amp;C Technologies, Inc\Desktop\Pers\TestRevenue (1)\TestRevenue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7CBF98-AE28-4F0D-87E3-52170DB502D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F406688-4E57-4456-8A38-4AA54D9A65BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" firstSheet="11" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -629,21 +629,21 @@
     <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2762,7 +2762,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{266E58B1-D977-4AB2-8F0A-647A07442DE7}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2831,7 +2833,7 @@
         <v>116</v>
       </c>
       <c r="G3" s="21">
-        <v>1714.0900000000001</v>
+        <v>1714.09</v>
       </c>
       <c r="H3" s="20">
         <v>202201</v>
@@ -2863,7 +2865,7 @@
         <v>116</v>
       </c>
       <c r="G4" s="21">
-        <v>-237.96500000000003</v>
+        <v>-237.9648</v>
       </c>
       <c r="H4" s="20">
         <v>202201</v>
@@ -2895,7 +2897,7 @@
         <v>116</v>
       </c>
       <c r="G5" s="21">
-        <v>-1357.143</v>
+        <v>-1357.1429000000001</v>
       </c>
       <c r="H5" s="20">
         <v>202201</v>
@@ -2927,7 +2929,7 @@
         <v>116</v>
       </c>
       <c r="G6" s="21">
-        <v>-118.98250000000002</v>
+        <v>-118.9824</v>
       </c>
       <c r="H6" s="20">
         <v>202201</v>
@@ -2991,7 +2993,7 @@
         <v>116</v>
       </c>
       <c r="G8" s="21">
-        <v>-1714.0900000000001</v>
+        <v>-1714.09</v>
       </c>
       <c r="H8" s="20">
         <v>202202</v>
@@ -3023,7 +3025,7 @@
         <v>116</v>
       </c>
       <c r="G9" s="21">
-        <v>-416.43799999999999</v>
+        <v>-416.43830000000003</v>
       </c>
       <c r="H9" s="20">
         <v>202202</v>
@@ -3055,7 +3057,7 @@
         <v>116</v>
       </c>
       <c r="G10" s="21">
-        <v>-208.21899999999999</v>
+        <v>-208.2192</v>
       </c>
       <c r="H10" s="20">
         <v>202202</v>
@@ -3087,7 +3089,7 @@
         <v>116</v>
       </c>
       <c r="G11" s="21">
-        <v>-461.05700000000002</v>
+        <v>-461.05680000000001</v>
       </c>
       <c r="H11" s="20">
         <v>202203</v>
@@ -3119,7 +3121,7 @@
         <v>116</v>
       </c>
       <c r="G12" s="21">
-        <v>-230.52850000000001</v>
+        <v>-230.5283</v>
       </c>
       <c r="H12" s="20">
         <v>202203</v>
@@ -3151,7 +3153,7 @@
         <v>116</v>
       </c>
       <c r="G13" s="21">
-        <v>-482.71349999999995</v>
+        <v>-482.71359999999999</v>
       </c>
       <c r="H13" s="20">
         <v>202204</v>
@@ -3215,7 +3217,7 @@
         <v>116</v>
       </c>
       <c r="G15" s="21">
-        <v>-1040.4434999999999</v>
+        <v>-1040.4436000000001</v>
       </c>
       <c r="H15" s="20">
         <v>202204</v>
@@ -3279,7 +3281,7 @@
         <v>116</v>
       </c>
       <c r="G17" s="21">
-        <v>-471.8415</v>
+        <v>-471.8417</v>
       </c>
       <c r="H17" s="20">
         <v>202205</v>
@@ -3311,7 +3313,7 @@
         <v>116</v>
       </c>
       <c r="G18" s="21">
-        <v>-471.8415</v>
+        <v>-471.8417</v>
       </c>
       <c r="H18" s="20">
         <v>202205</v>
@@ -3337,7 +3339,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E433FD4-1CD7-4287-A08F-AE9EDE2DEA08}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3398,10 +3402,10 @@
         <v>0</v>
       </c>
       <c r="F3" s="10">
-        <v>1714.0900000000001</v>
+        <v>1714.09</v>
       </c>
       <c r="G3" s="1">
-        <v>1714.0900000000001</v>
+        <v>1714.09</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3421,10 +3425,10 @@
         <v>0</v>
       </c>
       <c r="F4" s="10">
-        <v>1714.0900000000001</v>
+        <v>1714.09</v>
       </c>
       <c r="G4" s="1">
-        <v>1714.0900000000001</v>
+        <v>1714.09</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3444,10 +3448,10 @@
         <v>0</v>
       </c>
       <c r="F5" s="10">
-        <v>-237.96500000000003</v>
+        <v>-237.9648</v>
       </c>
       <c r="G5" s="1">
-        <v>-237.96500000000003</v>
+        <v>-237.9648</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3467,10 +3471,10 @@
         <v>0</v>
       </c>
       <c r="F6" s="1">
-        <v>-237.96500000000003</v>
+        <v>-237.9648</v>
       </c>
       <c r="G6" s="1">
-        <v>-237.96500000000003</v>
+        <v>-237.9648</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3490,10 +3494,10 @@
         <v>0</v>
       </c>
       <c r="F7" s="10">
-        <v>-1357.143</v>
+        <v>-1357.1429000000001</v>
       </c>
       <c r="G7" s="1">
-        <v>-1357.143</v>
+        <v>-1357.1429000000001</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3513,10 +3517,10 @@
         <v>0</v>
       </c>
       <c r="F8" s="10">
-        <v>-1357.143</v>
+        <v>-1357.1429000000001</v>
       </c>
       <c r="G8" s="1">
-        <v>-1357.143</v>
+        <v>-1357.1429000000001</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3536,10 +3540,10 @@
         <v>0</v>
       </c>
       <c r="F9" s="10">
-        <v>-118.98250000000002</v>
+        <v>-118.9824</v>
       </c>
       <c r="G9" s="1">
-        <v>-118.98250000000002</v>
+        <v>-118.9824</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3559,10 +3563,10 @@
         <v>0</v>
       </c>
       <c r="F10" s="10">
-        <v>-118.98250000000002</v>
+        <v>-118.9824</v>
       </c>
       <c r="G10" s="1">
-        <v>-118.98250000000002</v>
+        <v>-118.9824</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3648,13 +3652,13 @@
         <v>116</v>
       </c>
       <c r="E14" s="1">
-        <v>-237.96500000000003</v>
+        <v>-237.9648</v>
       </c>
       <c r="F14" s="1">
-        <v>-416.43799999999999</v>
+        <v>-416.43830000000003</v>
       </c>
       <c r="G14" s="1">
-        <v>-654.40300000000002</v>
+        <v>-654.40309999999999</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3671,13 +3675,13 @@
         <v>116</v>
       </c>
       <c r="E15" s="1">
-        <v>-237.96500000000003</v>
+        <v>-237.9648</v>
       </c>
       <c r="F15" s="1">
-        <v>-416.43799999999999</v>
+        <v>-416.43830000000003</v>
       </c>
       <c r="G15" s="1">
-        <v>-654.40300000000002</v>
+        <v>-654.40309999999999</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3694,13 +3698,13 @@
         <v>116</v>
       </c>
       <c r="E16" s="1">
-        <v>-1357.143</v>
+        <v>-1357.1429000000001</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
       </c>
       <c r="G16" s="1">
-        <v>-1357.143</v>
+        <v>-1357.1429000000001</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3717,13 +3721,13 @@
         <v>116</v>
       </c>
       <c r="E17" s="1">
-        <v>-1357.143</v>
+        <v>-1357.1429000000001</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
       </c>
       <c r="G17" s="1">
-        <v>-1357.143</v>
+        <v>-1357.1429000000001</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3740,13 +3744,13 @@
         <v>116</v>
       </c>
       <c r="E18" s="1">
-        <v>-118.98250000000002</v>
+        <v>-118.9824</v>
       </c>
       <c r="F18" s="1">
-        <v>-208.21899999999999</v>
+        <v>-208.2192</v>
       </c>
       <c r="G18" s="1">
-        <v>-327.20150000000001</v>
+        <v>-327.20159999999998</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3763,13 +3767,13 @@
         <v>116</v>
       </c>
       <c r="E19" s="1">
-        <v>-118.98250000000002</v>
+        <v>-118.9824</v>
       </c>
       <c r="F19" s="1">
-        <v>-208.21899999999999</v>
+        <v>-208.2192</v>
       </c>
       <c r="G19" s="1">
-        <v>-327.20150000000001</v>
+        <v>-327.20159999999998</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3855,13 +3859,13 @@
         <v>116</v>
       </c>
       <c r="E23" s="1">
-        <v>-654.40299999999991</v>
+        <v>-654.40309999999999</v>
       </c>
       <c r="F23" s="1">
-        <v>-461.05700000000002</v>
+        <v>-461.05680000000001</v>
       </c>
       <c r="G23" s="1">
-        <v>-1115.46</v>
+        <v>-1115.4599000000001</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3878,13 +3882,13 @@
         <v>116</v>
       </c>
       <c r="E24" s="1">
-        <v>-654.40299999999991</v>
+        <v>-654.40309999999999</v>
       </c>
       <c r="F24" s="1">
-        <v>-461.05700000000002</v>
+        <v>-461.05680000000001</v>
       </c>
       <c r="G24" s="1">
-        <v>-1115.46</v>
+        <v>-1115.4599000000001</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3901,13 +3905,13 @@
         <v>116</v>
       </c>
       <c r="E25" s="1">
-        <v>-1357.143</v>
+        <v>-1357.1429000000001</v>
       </c>
       <c r="F25" s="1">
         <v>0</v>
       </c>
       <c r="G25" s="1">
-        <v>-1357.143</v>
+        <v>-1357.1429000000001</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3924,13 +3928,13 @@
         <v>116</v>
       </c>
       <c r="E26" s="1">
-        <v>-1357.143</v>
+        <v>-1357.1429000000001</v>
       </c>
       <c r="F26" s="1">
         <v>0</v>
       </c>
       <c r="G26" s="1">
-        <v>-1357.143</v>
+        <v>-1357.1429000000001</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3947,13 +3951,13 @@
         <v>116</v>
       </c>
       <c r="E27" s="1">
-        <v>-327.20149999999995</v>
+        <v>-327.20159999999998</v>
       </c>
       <c r="F27" s="1">
-        <v>-230.52850000000001</v>
+        <v>-230.5283</v>
       </c>
       <c r="G27" s="1">
-        <v>-557.73</v>
+        <v>-557.72990000000004</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3970,13 +3974,13 @@
         <v>116</v>
       </c>
       <c r="E28" s="1">
-        <v>-327.20149999999995</v>
+        <v>-327.20159999999998</v>
       </c>
       <c r="F28" s="1">
-        <v>-230.52850000000001</v>
+        <v>-230.5283</v>
       </c>
       <c r="G28" s="1">
-        <v>-557.73</v>
+        <v>-557.72990000000004</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4062,10 +4066,10 @@
         <v>116</v>
       </c>
       <c r="E32" s="1">
-        <v>-1115.46</v>
+        <v>-1115.4599000000001</v>
       </c>
       <c r="F32" s="1">
-        <v>-482.71349999999995</v>
+        <v>-482.71359999999999</v>
       </c>
       <c r="G32" s="1">
         <v>-1598.1735000000001</v>
@@ -4085,10 +4089,10 @@
         <v>116</v>
       </c>
       <c r="E33" s="1">
-        <v>-1115.46</v>
+        <v>-1115.4599000000001</v>
       </c>
       <c r="F33" s="1">
-        <v>-482.71349999999995</v>
+        <v>-482.71359999999999</v>
       </c>
       <c r="G33" s="1">
         <v>-1598.1735000000001</v>
@@ -4108,13 +4112,13 @@
         <v>116</v>
       </c>
       <c r="E34" s="1">
-        <v>-1357.143</v>
+        <v>-1357.1429000000001</v>
       </c>
       <c r="F34" s="1">
         <v>-31.745999999999999</v>
       </c>
       <c r="G34" s="1">
-        <v>-1388.8890000000001</v>
+        <v>-1388.8888999999999</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4131,13 +4135,13 @@
         <v>116</v>
       </c>
       <c r="E35" s="1">
-        <v>-1357.143</v>
+        <v>-1357.1429000000001</v>
       </c>
       <c r="F35" s="1">
         <v>-31.745999999999999</v>
       </c>
       <c r="G35" s="1">
-        <v>-1388.8890000000001</v>
+        <v>-1388.8888999999999</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4154,10 +4158,10 @@
         <v>116</v>
       </c>
       <c r="E36" s="1">
-        <v>-557.73</v>
+        <v>-557.72990000000004</v>
       </c>
       <c r="F36" s="1">
-        <v>-1040.4434999999999</v>
+        <v>-1040.4436000000001</v>
       </c>
       <c r="G36" s="1">
         <v>-1598.1735000000001</v>
@@ -4177,10 +4181,10 @@
         <v>116</v>
       </c>
       <c r="E37" s="1">
-        <v>-557.73</v>
+        <v>-557.72990000000004</v>
       </c>
       <c r="F37" s="1">
-        <v>-1040.4434999999999</v>
+        <v>-1040.4436000000001</v>
       </c>
       <c r="G37" s="1">
         <v>-1598.1735000000001</v>
@@ -4272,10 +4276,10 @@
         <v>-1598.1735000000001</v>
       </c>
       <c r="F41" s="1">
-        <v>-471.8415</v>
+        <v>-471.8417</v>
       </c>
       <c r="G41" s="1">
-        <v>-2070.0150000000003</v>
+        <v>-2070.0151999999998</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4295,10 +4299,10 @@
         <v>-1598.1735000000001</v>
       </c>
       <c r="F42" s="1">
-        <v>-471.8415</v>
+        <v>-471.8417</v>
       </c>
       <c r="G42" s="1">
-        <v>-2070.0150000000003</v>
+        <v>-2070.0151999999998</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4315,13 +4319,13 @@
         <v>116</v>
       </c>
       <c r="E43" s="1">
-        <v>-1388.8890000000001</v>
+        <v>-1388.8888999999999</v>
       </c>
       <c r="F43" s="1">
         <v>0</v>
       </c>
       <c r="G43" s="1">
-        <v>-1388.8890000000001</v>
+        <v>-1388.8888999999999</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4338,13 +4342,13 @@
         <v>116</v>
       </c>
       <c r="E44" s="1">
-        <v>-1388.8890000000001</v>
+        <v>-1388.8888999999999</v>
       </c>
       <c r="F44" s="1">
         <v>0</v>
       </c>
       <c r="G44" s="1">
-        <v>-1388.8890000000001</v>
+        <v>-1388.8888999999999</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4364,10 +4368,10 @@
         <v>-1598.1735000000001</v>
       </c>
       <c r="F45" s="1">
-        <v>-471.8415</v>
+        <v>-471.8417</v>
       </c>
       <c r="G45" s="1">
-        <v>-2070.0150000000003</v>
+        <v>-2070.0151999999998</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4387,10 +4391,10 @@
         <v>-1598.1735000000001</v>
       </c>
       <c r="F46" s="1">
-        <v>-471.8415</v>
+        <v>-471.8417</v>
       </c>
       <c r="G46" s="1">
-        <v>-2070.0150000000003</v>
+        <v>-2070.0151999999998</v>
       </c>
     </row>
   </sheetData>
@@ -4457,13 +4461,13 @@
         <v>116</v>
       </c>
       <c r="D3" s="23">
-        <v>-5.0000000004501999E-4</v>
+        <v>-1E-4</v>
       </c>
       <c r="E3" s="23">
         <v>0</v>
       </c>
       <c r="F3" s="23">
-        <v>-5.0000000004501999E-4</v>
+        <v>-1E-4</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4477,13 +4481,13 @@
         <v>116</v>
       </c>
       <c r="D4" s="23">
-        <v>-1714.0905000000002</v>
+        <v>-1714.0900999999999</v>
       </c>
       <c r="E4" s="23">
         <v>0</v>
       </c>
       <c r="F4" s="23">
-        <v>-1714.0905000000002</v>
+        <v>-1714.0900999999999</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4497,13 +4501,13 @@
         <v>116</v>
       </c>
       <c r="D5" s="23">
-        <v>1714.0900000000001</v>
+        <v>1714.09</v>
       </c>
       <c r="E5" s="23">
         <v>0</v>
       </c>
       <c r="F5" s="23">
-        <v>1714.0900000000001</v>
+        <v>1714.09</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4537,13 +4541,13 @@
         <v>116</v>
       </c>
       <c r="D7" s="23">
-        <v>7161.2529999999997</v>
+        <v>7161.2524999999996</v>
       </c>
       <c r="E7" s="23">
-        <v>-5.0000000004501999E-4</v>
+        <v>-1E-4</v>
       </c>
       <c r="F7" s="23">
-        <v>7161.2524999999996</v>
+        <v>7161.2524000000003</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4557,13 +4561,13 @@
         <v>116</v>
       </c>
       <c r="D8" s="23">
-        <v>-624.65699999999993</v>
+        <v>-624.65750000000003</v>
       </c>
       <c r="E8" s="23">
-        <v>-1714.0905000000002</v>
+        <v>-1714.0900999999999</v>
       </c>
       <c r="F8" s="23">
-        <v>-2338.7474999999999</v>
+        <v>-2338.7476000000001</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4617,13 +4621,13 @@
         <v>116</v>
       </c>
       <c r="D11" s="23">
-        <v>-691.58550000000002</v>
+        <v>-691.58510000000001</v>
       </c>
       <c r="E11" s="23">
-        <v>7161.2524999999996</v>
+        <v>7161.2524000000003</v>
       </c>
       <c r="F11" s="23">
-        <v>6469.6670000000013</v>
+        <v>6469.6673000000001</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4637,13 +4641,13 @@
         <v>116</v>
       </c>
       <c r="D12" s="23">
-        <v>-691.58550000000002</v>
+        <v>-691.58510000000001</v>
       </c>
       <c r="E12" s="23">
-        <v>-2338.7474999999999</v>
+        <v>-2338.7476000000001</v>
       </c>
       <c r="F12" s="23">
-        <v>-3030.3330000000001</v>
+        <v>-3030.3326999999999</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4697,13 +4701,13 @@
         <v>116</v>
       </c>
       <c r="D15" s="23">
-        <v>-1554.9029999999998</v>
+        <v>-1554.9032</v>
       </c>
       <c r="E15" s="23">
-        <v>6469.6670000000013</v>
+        <v>6469.6673000000001</v>
       </c>
       <c r="F15" s="23">
-        <v>4914.7640000000001</v>
+        <v>4914.7641000000003</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4717,13 +4721,13 @@
         <v>116</v>
       </c>
       <c r="D16" s="23">
-        <v>-1554.9029999999998</v>
+        <v>-1554.9032</v>
       </c>
       <c r="E16" s="23">
-        <v>-3030.3330000000001</v>
+        <v>-3030.3326999999999</v>
       </c>
       <c r="F16" s="23">
-        <v>-4585.2359999999999</v>
+        <v>-4585.2358999999997</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4777,13 +4781,13 @@
         <v>116</v>
       </c>
       <c r="D19" s="23">
-        <v>2056.317</v>
+        <v>2056.3166000000001</v>
       </c>
       <c r="E19" s="23">
-        <v>4914.7640000000001</v>
+        <v>4914.7641000000003</v>
       </c>
       <c r="F19" s="23">
-        <v>6971.081000000001</v>
+        <v>6971.0807000000004</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4797,13 +4801,13 @@
         <v>116</v>
       </c>
       <c r="D20" s="23">
-        <v>-943.68299999999999</v>
+        <v>-943.68340000000001</v>
       </c>
       <c r="E20" s="23">
-        <v>-4585.2359999999999</v>
+        <v>-4585.2358999999997</v>
       </c>
       <c r="F20" s="23">
-        <v>-5528.9190000000008</v>
+        <v>-5528.9192999999996</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4838,7 +4842,7 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
@@ -4848,8 +4852,6 @@
     <col min="2" max="2" width="46.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="23.5703125" style="1" customWidth="1"/>
     <col min="4" max="5" width="24.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -4888,10 +4890,10 @@
         <v>0</v>
       </c>
       <c r="D3" s="1">
-        <v>-1.4999999994245172E-3</v>
+        <v>-2.0000000000000001E-4</v>
       </c>
       <c r="E3" s="1">
-        <v>-1.4999999994245172E-3</v>
+        <v>-2.0000000000000001E-4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -4905,10 +4907,10 @@
         <v>0</v>
       </c>
       <c r="D4" s="1">
-        <v>-5142.2715000000007</v>
+        <v>-5142.2701999999999</v>
       </c>
       <c r="E4" s="1">
-        <v>-5142.2715000000007</v>
+        <v>-5142.2701999999999</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -4953,13 +4955,13 @@
         <v>42</v>
       </c>
       <c r="C7" s="1">
-        <v>-1.5000000012435066E-3</v>
+        <v>-2.0000000000000001E-4</v>
       </c>
       <c r="D7" s="1">
-        <v>21483.759000000002</v>
+        <v>21483.7575</v>
       </c>
       <c r="E7" s="1">
-        <v>21483.7575</v>
+        <v>21483.757300000001</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4970,13 +4972,13 @@
         <v>34</v>
       </c>
       <c r="C8" s="1">
-        <v>-5142.2715000000007</v>
+        <v>-5142.2701999999999</v>
       </c>
       <c r="D8" s="1">
-        <v>-1873.9709999999998</v>
+        <v>-1873.9725000000001</v>
       </c>
       <c r="E8" s="1">
-        <v>-7016.2425000000003</v>
+        <v>-7016.2426999999998</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4987,10 +4989,10 @@
         <v>43</v>
       </c>
       <c r="C9" s="1">
-        <v>5142.2699999999995</v>
+        <v>5142.2700000000004</v>
       </c>
       <c r="D9" s="1">
-        <v>-5142.2699999999995</v>
+        <v>-5142.2700000000004</v>
       </c>
       <c r="E9" s="1">
         <v>0</v>
@@ -5021,13 +5023,13 @@
         <v>42</v>
       </c>
       <c r="C11" s="1">
-        <v>21483.7575</v>
+        <v>21483.757300000001</v>
       </c>
       <c r="D11" s="1">
-        <v>-2074.7565</v>
+        <v>-2074.7555000000002</v>
       </c>
       <c r="E11" s="1">
-        <v>19409.001</v>
+        <v>19409.001799999998</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5038,13 +5040,13 @@
         <v>34</v>
       </c>
       <c r="C12" s="1">
-        <v>-7016.2425000000003</v>
+        <v>-7016.2426999999998</v>
       </c>
       <c r="D12" s="1">
-        <v>-2074.7565</v>
+        <v>-2074.7555000000002</v>
       </c>
       <c r="E12" s="1">
-        <v>-9090.9989999999998</v>
+        <v>-9090.9982</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5089,13 +5091,13 @@
         <v>42</v>
       </c>
       <c r="C15" s="1">
-        <v>19409.001</v>
+        <v>19409.001799999998</v>
       </c>
       <c r="D15" s="1">
-        <v>-4664.7089999999998</v>
+        <v>-4664.7094999999999</v>
       </c>
       <c r="E15" s="1">
-        <v>14744.292000000003</v>
+        <v>14744.292299999999</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5106,13 +5108,13 @@
         <v>34</v>
       </c>
       <c r="C16" s="1">
-        <v>-9090.9989999999998</v>
+        <v>-9090.9982</v>
       </c>
       <c r="D16" s="1">
-        <v>-4664.7089999999998</v>
+        <v>-4664.7094999999999</v>
       </c>
       <c r="E16" s="1">
-        <v>-13755.708000000001</v>
+        <v>-13755.707700000001</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5157,13 +5159,13 @@
         <v>42</v>
       </c>
       <c r="C19" s="1">
-        <v>14744.292000000003</v>
+        <v>14744.292299999999</v>
       </c>
       <c r="D19" s="1">
-        <v>6168.9509999999973</v>
+        <v>6168.9498000000003</v>
       </c>
       <c r="E19" s="1">
-        <v>20913.243000000006</v>
+        <v>20913.242099999999</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5174,13 +5176,13 @@
         <v>34</v>
       </c>
       <c r="C20" s="1">
-        <v>-13755.708000000001</v>
+        <v>-13755.707700000001</v>
       </c>
       <c r="D20" s="1">
-        <v>-2831.049</v>
+        <v>-2831.0502000000001</v>
       </c>
       <c r="E20" s="1">
-        <v>-16586.757000000001</v>
+        <v>-16586.757900000001</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5859,13 +5861,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -5883,7 +5885,7 @@
       <c r="E2" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="L2" s="26" t="s">
+      <c r="L2" s="30" t="s">
         <v>84</v>
       </c>
       <c r="M2" s="12" t="s">
@@ -5921,7 +5923,7 @@
       <c r="E3" s="7">
         <v>0</v>
       </c>
-      <c r="L3" s="26"/>
+      <c r="L3" s="30"/>
       <c r="M3" s="7" t="s">
         <v>93</v>
       </c>
@@ -5955,7 +5957,7 @@
         <v>96</v>
       </c>
       <c r="E4" s="7"/>
-      <c r="L4" s="26"/>
+      <c r="L4" s="30"/>
       <c r="M4" s="7" t="s">
         <v>93</v>
       </c>
@@ -6032,16 +6034,16 @@
       <c r="E8" s="7"/>
     </row>
     <row r="11" spans="1:18" ht="21" x14ac:dyDescent="0.35">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
     </row>
     <row r="12" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
@@ -6200,10 +6202,10 @@
       <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="B18" s="28"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="17">
         <f>SUM(C13:C17)</f>
         <v>1900</v>
@@ -6224,11 +6226,11 @@
       <c r="H18" s="7"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B21" s="18" t="s">
@@ -6422,11 +6424,11 @@
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B38" s="29" t="s">
+      <c r="B38" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="18" t="s">
@@ -6620,33 +6622,33 @@
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A55" s="30" t="s">
+      <c r="A55" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="B55" s="30"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="30"/>
-      <c r="F55" s="30"/>
-      <c r="G55" s="30"/>
-      <c r="H55" s="30"/>
-      <c r="I55" s="30"/>
-      <c r="J55" s="30"/>
-      <c r="K55" s="30"/>
-      <c r="L55" s="30"/>
-      <c r="M55" s="30"/>
-      <c r="N55" s="30"/>
-      <c r="O55" s="30"/>
-      <c r="P55" s="30"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="26"/>
+      <c r="G55" s="26"/>
+      <c r="H55" s="26"/>
+      <c r="I55" s="26"/>
+      <c r="J55" s="26"/>
+      <c r="K55" s="26"/>
+      <c r="L55" s="26"/>
+      <c r="M55" s="26"/>
+      <c r="N55" s="26"/>
+      <c r="O55" s="26"/>
+      <c r="P55" s="26"/>
     </row>
     <row r="57" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A57" s="25" t="s">
+      <c r="A57" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="B57" s="25"/>
-      <c r="C57" s="25"/>
-      <c r="D57" s="25"/>
-      <c r="E57" s="25"/>
+      <c r="B57" s="27"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="27"/>
     </row>
     <row r="58" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
@@ -6754,16 +6756,16 @@
       <c r="E64" s="7"/>
     </row>
     <row r="67" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A67" s="27" t="s">
+      <c r="A67" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="B67" s="27"/>
-      <c r="C67" s="27"/>
-      <c r="D67" s="27"/>
-      <c r="E67" s="27"/>
-      <c r="F67" s="27"/>
-      <c r="G67" s="27"/>
-      <c r="H67" s="27"/>
+      <c r="B67" s="28"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="28"/>
+      <c r="E67" s="28"/>
+      <c r="F67" s="28"/>
+      <c r="G67" s="28"/>
+      <c r="H67" s="28"/>
     </row>
     <row r="68" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
@@ -6922,10 +6924,10 @@
       <c r="H73" s="7"/>
     </row>
     <row r="74" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A74" s="28" t="s">
+      <c r="A74" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="B74" s="28"/>
+      <c r="B74" s="29"/>
       <c r="C74" s="17">
         <f>SUM(C69:C73)</f>
         <v>2500</v>
@@ -6946,11 +6948,11 @@
       <c r="H74" s="7"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B76" s="29" t="s">
+      <c r="B76" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="C76" s="29"/>
-      <c r="D76" s="29"/>
+      <c r="C76" s="25"/>
+      <c r="D76" s="25"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B77" s="18" t="s">
@@ -7144,11 +7146,11 @@
       </c>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B94" s="29" t="s">
+      <c r="B94" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="C94" s="29"/>
-      <c r="D94" s="29"/>
+      <c r="C94" s="25"/>
+      <c r="D94" s="25"/>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B95" s="18" t="s">
@@ -7343,6 +7345,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="B20:D20"/>
     <mergeCell ref="B76:D76"/>
     <mergeCell ref="B94:D94"/>
     <mergeCell ref="B38:D38"/>
@@ -7350,11 +7357,6 @@
     <mergeCell ref="A57:E57"/>
     <mergeCell ref="A67:H67"/>
     <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="L2:L4"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="B20:D20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -7365,7 +7367,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>